<commit_message>
Fix Id 29 e 37
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/SUITE_LOG80/1.0/report-checklist.xlsx
@@ -427,22 +427,7 @@
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.70073af09e34df4005c52f39dece35c5f7521e873bbb0710cb5a3ee0117438ec.f1d3da9f95^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-02-16T10:56:24Z</t>
-  </si>
-  <si>
-    <t>383487740e40dc1d</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>2023-02-16T10:58:05Z</t>
-  </si>
-  <si>
-    <t>d5d25318ad4b2383</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.70073af09e34df4005c52f39dece35c5f7521e873bbb0710cb5a3ee0117438ec.335aeffdf1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-02-16T10:59:43Z</t>
@@ -518,6 +503,21 @@
   </si>
   <si>
     <t>2023-02-16T11:35:48Z</t>
+  </si>
+  <si>
+    <t>2023-02-22T11:41:33Z</t>
+  </si>
+  <si>
+    <t>023903a089c98977</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.31ddfdfedf10087dbe67c4d0c960b3996be1bf5a42cfa33a4e268c8ee80d99e3.aa1c80e57b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>c7476a627ecb17c0</t>
+  </si>
+  <si>
+    <t>2023-02-22T11:45:05Z</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -817,9 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1157,10 +1154,10 @@
   <dimension ref="A1:O873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1196,12 +1193,12 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="18.75">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="26"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1214,14 +1211,14 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="26"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1234,12 +1231,12 @@
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" ht="15.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1253,12 +1250,12 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="26"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1271,8 +1268,8 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="6"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1372,31 +1369,31 @@
       <c r="D10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>44973</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16" t="s">
+      <c r="J10" s="15"/>
+      <c r="K10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="18"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" ht="75.75" thickBot="1">
       <c r="A11" s="11">
@@ -1411,31 +1408,31 @@
       <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>44973</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16" t="s">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="18"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" ht="75.75" thickBot="1">
       <c r="A12" s="11">
@@ -1450,31 +1447,31 @@
       <c r="D12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>44973</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16" t="s">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="18"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" ht="75.75" thickBot="1">
       <c r="A13" s="11">
@@ -1489,23 +1486,23 @@
       <c r="D13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16" t="s">
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="18"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" ht="90.75" thickBot="1">
       <c r="A14" s="11">
@@ -1520,35 +1517,35 @@
       <c r="D14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="14">
-        <v>44973</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="13">
+        <v>44979</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="17" t="s">
+      <c r="M14" s="15"/>
+      <c r="N14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:15" ht="105.75" thickBot="1">
       <c r="A15" s="11">
@@ -1563,35 +1560,35 @@
       <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="14">
-        <v>44973</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="16" t="s">
+      <c r="F15" s="13">
+        <v>44979</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="17" t="s">
+      <c r="M15" s="15"/>
+      <c r="N15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="18"/>
+      <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="11">
@@ -1606,31 +1603,31 @@
       <c r="D16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>44973</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16" t="s">
+      <c r="G16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="17" t="s">
+      <c r="M16" s="15"/>
+      <c r="N16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="18"/>
+      <c r="O16" s="17"/>
     </row>
     <row r="17" spans="1:15" ht="75.75" thickBot="1">
       <c r="A17" s="11">
@@ -1645,35 +1642,35 @@
       <c r="D17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>44973</v>
       </c>
-      <c r="G17" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="J17" s="16" t="s">
+      <c r="G17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="K17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17" t="s">
+      <c r="M17" s="15"/>
+      <c r="N17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="18"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="1:15" ht="75.75" thickBot="1">
       <c r="A18" s="11">
@@ -1688,35 +1685,35 @@
       <c r="D18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>44973</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="16" t="s">
+      <c r="G18" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="L18" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17" t="s">
+      <c r="M18" s="15"/>
+      <c r="N18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O18" s="18" t="s">
+      <c r="O18" s="17" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1733,35 +1730,35 @@
       <c r="D19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <v>44973</v>
       </c>
-      <c r="G19" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="16" t="s">
+      <c r="G19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="K19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M19" s="15"/>
+      <c r="N19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O19" s="18"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" ht="75.75" thickBot="1">
       <c r="A20" s="11">
@@ -1776,25 +1773,25 @@
       <c r="D20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O20" s="18"/>
+      <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" ht="75.75" thickBot="1">
       <c r="A21" s="11">
@@ -1809,35 +1806,35 @@
       <c r="D21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="13">
         <v>44973</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="J21" s="16" t="s">
+      <c r="G21" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="K21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17" t="s">
+      <c r="M21" s="15"/>
+      <c r="N21" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="18"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" ht="75.75" thickBot="1">
       <c r="A22" s="11">
@@ -1852,35 +1849,35 @@
       <c r="D22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="13">
         <v>44973</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" s="16" t="s">
+      <c r="G22" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="17" t="s">
+      <c r="M22" s="15"/>
+      <c r="N22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O22" s="18"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" ht="75.75" thickBot="1">
       <c r="A23" s="11">
@@ -1895,35 +1892,35 @@
       <c r="D23" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="13">
         <v>44973</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J23" s="16" t="s">
+      <c r="G23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="16" t="s">
+      <c r="K23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="17" t="s">
+      <c r="M23" s="15"/>
+      <c r="N23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="18"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" ht="75.75" thickBot="1">
       <c r="A24" s="11">
@@ -1938,35 +1935,35 @@
       <c r="D24" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="13">
         <v>44973</v>
       </c>
-      <c r="G24" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J24" s="16" t="s">
+      <c r="G24" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="K24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="16" t="s">
+      <c r="L24" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="17" t="s">
+      <c r="M24" s="15"/>
+      <c r="N24" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="18"/>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" spans="1:15" ht="75.75" thickBot="1">
       <c r="A25" s="11">
@@ -1981,25 +1978,25 @@
       <c r="D25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16" t="s">
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="17" t="s">
+      <c r="N25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" ht="75.75" thickBot="1">
       <c r="A26" s="11">
@@ -2014,25 +2011,25 @@
       <c r="D26" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16" t="s">
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16" t="s">
+      <c r="L26" s="15"/>
+      <c r="M26" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="17" t="s">
+      <c r="N26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="18"/>
+      <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" ht="75.75" thickBot="1">
       <c r="A27" s="11">
@@ -2047,33 +2044,33 @@
       <c r="D27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="13">
         <v>44973</v>
       </c>
-      <c r="G27" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="J27" s="16" t="s">
+      <c r="G27" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="16" t="s">
+      <c r="K27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17" t="s">
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O27" s="18"/>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:15" ht="75">
       <c r="A28" s="11">
@@ -2088,25 +2085,25 @@
       <c r="D28" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16" t="s">
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16" t="s">
+      <c r="L28" s="15"/>
+      <c r="M28" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="N28" s="17" t="s">
+      <c r="N28" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O28" s="18"/>
+      <c r="O28" s="17"/>
     </row>
     <row r="29" spans="1:15">
       <c r="F29" s="2"/>
@@ -12287,26 +12284,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>